<commit_message>
23634 and 23635 scripts added
</commit_message>
<xml_diff>
--- a/Q2Mobile_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2Mobile_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="116">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -367,6 +367,15 @@
   </si>
   <si>
     <t>C24233_VerifyMultipleAccountAddressChange</t>
+  </si>
+  <si>
+    <t>C23629_VerifyStopPaymentViaServices</t>
+  </si>
+  <si>
+    <t>C23635_VerifyTDECURatesViaServices</t>
+  </si>
+  <si>
+    <t>C23634_VerifyCreditCardInformationViaServices</t>
   </si>
 </sst>
 </file>
@@ -740,7 +749,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -748,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,6 +1574,69 @@
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>112</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1615,9 +1687,13 @@
     <hyperlink ref="E45" r:id="rId44"/>
     <hyperlink ref="E46" r:id="rId45"/>
     <hyperlink ref="E47" r:id="rId46"/>
+    <hyperlink ref="E48" r:id="rId47"/>
+    <hyperlink ref="E49" r:id="rId48"/>
+    <hyperlink ref="E50" r:id="rId49"/>
+    <hyperlink ref="E51" r:id="rId50"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId47"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
 
@@ -1625,7 +1701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
C24239 and C24240 scripts added
</commit_message>
<xml_diff>
--- a/Q2Mobile_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2Mobile_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="118">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -376,6 +376,12 @@
   </si>
   <si>
     <t>C23634_VerifyCreditCardInformationViaServices</t>
+  </si>
+  <si>
+    <t>C24239_VerifyAllAccountsAddressChange</t>
+  </si>
+  <si>
+    <t>C24240_VerifyAddressChangeSuccessMessage</t>
   </si>
 </sst>
 </file>
@@ -749,7 +755,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -757,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51:F51"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,6 +1642,40 @@
         <v>33</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1691,18 +1731,20 @@
     <hyperlink ref="E49" r:id="rId48"/>
     <hyperlink ref="E50" r:id="rId49"/>
     <hyperlink ref="E51" r:id="rId50"/>
+    <hyperlink ref="E52" r:id="rId51"/>
+    <hyperlink ref="E53" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId51"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId53"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,6 +2101,14 @@
       </c>
       <c r="C18" s="5" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
24242 and 24243 scripts added
</commit_message>
<xml_diff>
--- a/Q2Mobile_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2Mobile_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="Alerts" sheetId="3" r:id="rId3"/>
-    <sheet name="Address" sheetId="4" r:id="rId4"/>
+    <sheet name="StopPayment" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="128">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -382,6 +382,36 @@
   </si>
   <si>
     <t>C24240_VerifyAddressChangeSuccessMessage</t>
+  </si>
+  <si>
+    <t>C23630_VerifySingleCheckStopPaymentCreation</t>
+  </si>
+  <si>
+    <t>C23631_VerifyMultipleCheckStopPaymentCreation</t>
+  </si>
+  <si>
+    <t>C24242_VerifyChangeAddressRequestOnActivityCenterPage</t>
+  </si>
+  <si>
+    <t>C24243_VerifyChangeAddressRequestInquiryOnActivityCenterPage</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>Payee</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>EndCheckNumber</t>
+  </si>
+  <si>
+    <t>abcdefghijklmnopqrstuvwxyz1234567890abcde</t>
+  </si>
+  <si>
+    <t>456789123</t>
   </si>
 </sst>
 </file>
@@ -755,7 +785,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -763,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,6 +1706,74 @@
         <v>33</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" t="s">
+        <v>33</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1733,18 +1831,22 @@
     <hyperlink ref="E51" r:id="rId50"/>
     <hyperlink ref="E52" r:id="rId51"/>
     <hyperlink ref="E53" r:id="rId52"/>
+    <hyperlink ref="E54" r:id="rId53"/>
+    <hyperlink ref="E55" r:id="rId54"/>
+    <hyperlink ref="E56" r:id="rId55"/>
+    <hyperlink ref="E57" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId53"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,6 +2210,22 @@
         <v>117</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2399,12 +2517,76 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q2 mobile scripts committed
</commit_message>
<xml_diff>
--- a/Q2Mobile_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2Mobile_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Alerts" sheetId="3" r:id="rId3"/>
     <sheet name="StopPayment" sheetId="4" r:id="rId4"/>
     <sheet name="WireTransfer" sheetId="5" r:id="rId5"/>
+    <sheet name="Location" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="186">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -79,12 +80,6 @@
     <t>VerifyLoginValidUsernamePassword</t>
   </si>
   <si>
-    <t>user50225500</t>
-  </si>
-  <si>
-    <t>Kony@1234</t>
-  </si>
-  <si>
     <t>VerifyPSCUCreditCard</t>
   </si>
   <si>
@@ -106,12 +101,6 @@
     <t>C23548_VerifyLoginWithInValidPassword</t>
   </si>
   <si>
-    <t>user502255w</t>
-  </si>
-  <si>
-    <t>Kony@12354</t>
-  </si>
-  <si>
     <t>C23552_VerifyRegisterMyDeviceOption</t>
   </si>
   <si>
@@ -130,9 +119,6 @@
     <t>C23745_VerifyActivityCenter</t>
   </si>
   <si>
-    <t>user2046417</t>
-  </si>
-  <si>
     <t>C23686_VerifyFundTransferOption</t>
   </si>
   <si>
@@ -316,9 +302,6 @@
     <t>Available Balance</t>
   </si>
   <si>
-    <t>greater than</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -355,9 +338,6 @@
     <t>6712437832</t>
   </si>
   <si>
-    <t>Text Message</t>
-  </si>
-  <si>
     <t>Birthday</t>
   </si>
   <si>
@@ -472,13 +452,142 @@
     <t>Texas</t>
   </si>
   <si>
-    <t>75643</t>
-  </si>
-  <si>
     <t>C23654_VerifyWireTransferRecipientCreation</t>
   </si>
   <si>
     <t>C23636_VerifyMobileDepositEnrollOption</t>
+  </si>
+  <si>
+    <t>C23632_VerifySendingSingleCheckStopPayment</t>
+  </si>
+  <si>
+    <t>C23633_VerifySendingMultipleCheckStopPayment</t>
+  </si>
+  <si>
+    <t>75075</t>
+  </si>
+  <si>
+    <t>C23655_VerifyAddingMultipleAccountsToWireTransferRecipient</t>
+  </si>
+  <si>
+    <t>C23570_VerifyMapOfLocations</t>
+  </si>
+  <si>
+    <t>LocName</t>
+  </si>
+  <si>
+    <t>LocAddress</t>
+  </si>
+  <si>
+    <t>ATM Name</t>
+  </si>
+  <si>
+    <t>ATMAddress</t>
+  </si>
+  <si>
+    <t>InTouch CU</t>
+  </si>
+  <si>
+    <t>4701 W Plano Pkwy Ste 100</t>
+  </si>
+  <si>
+    <t>Walgreens</t>
+  </si>
+  <si>
+    <t>2001 Custer Rd</t>
+  </si>
+  <si>
+    <t>C23573_VerifyLocationSearch</t>
+  </si>
+  <si>
+    <t>50225500</t>
+  </si>
+  <si>
+    <t>2046417</t>
+  </si>
+  <si>
+    <t>Kony@567</t>
+  </si>
+  <si>
+    <t>2046417100</t>
+  </si>
+  <si>
+    <t>Test@546</t>
+  </si>
+  <si>
+    <t>10225500</t>
+  </si>
+  <si>
+    <t>Kony@566</t>
+  </si>
+  <si>
+    <t>-2046417</t>
+  </si>
+  <si>
+    <t>-50225500</t>
+  </si>
+  <si>
+    <t>Reminder</t>
+  </si>
+  <si>
+    <t>More Than</t>
+  </si>
+  <si>
+    <t>-2445</t>
+  </si>
+  <si>
+    <t>Kony@123</t>
+  </si>
+  <si>
+    <t>C25043_VerifyOneTimeLoanPaymentSetup</t>
+  </si>
+  <si>
+    <t>70024450</t>
+  </si>
+  <si>
+    <t>927878595</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>consumer loan payoff</t>
+  </si>
+  <si>
+    <t>C25044_VerifyRecurringLoanPaymentSetup</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>C25036_VerifyLoanPaymentOption</t>
+  </si>
+  <si>
+    <t>C25045_VerifyRegularMortageLoanPayment</t>
+  </si>
+  <si>
+    <t>C25038_VerifyRegularCommercialLoanPayment</t>
+  </si>
+  <si>
+    <t>2445058</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Mortage loan</t>
+  </si>
+  <si>
+    <t>Voice</t>
+  </si>
+  <si>
+    <t>SMS Text Message</t>
+  </si>
+  <si>
+    <t>-72101</t>
+  </si>
+  <si>
+    <t>Kony@111</t>
   </si>
 </sst>
 </file>
@@ -860,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,16 +1011,16 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
+      <c r="D2" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -919,16 +1028,16 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
+      <c r="D3" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -936,16 +1045,16 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>16</v>
+      <c r="D4" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -953,16 +1062,16 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>16</v>
+      <c r="D5" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -970,16 +1079,16 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>16</v>
+      <c r="D6" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -987,16 +1096,16 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
+      <c r="D7" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -1004,16 +1113,16 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
-        <v>25</v>
+      <c r="D8" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1021,16 +1130,16 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" t="s">
-        <v>16</v>
+      <c r="D9" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>26</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -1038,16 +1147,16 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" t="s">
-        <v>16</v>
+      <c r="D10" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -1055,16 +1164,16 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" t="s">
-        <v>16</v>
+      <c r="D11" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -1072,16 +1181,16 @@
       <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" t="s">
-        <v>16</v>
+      <c r="D12" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1089,16 +1198,16 @@
       <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" t="s">
-        <v>16</v>
+      <c r="D13" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -1106,16 +1215,16 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
-        <v>16</v>
+      <c r="D14" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -1123,16 +1232,16 @@
       <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="D15" t="s">
-        <v>33</v>
+      <c r="D15" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -1140,16 +1249,16 @@
       <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D16" t="s">
-        <v>33</v>
+      <c r="D16" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -1157,16 +1266,16 @@
       <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="D17" t="s">
-        <v>33</v>
+      <c r="D17" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -1174,16 +1283,16 @@
       <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="D18" t="s">
-        <v>33</v>
+      <c r="D18" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -1191,16 +1300,16 @@
       <c r="C19" t="s">
         <v>12</v>
       </c>
-      <c r="D19" t="s">
-        <v>33</v>
+      <c r="D19" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -1208,16 +1317,16 @@
       <c r="C20" t="s">
         <v>12</v>
       </c>
-      <c r="D20" t="s">
-        <v>33</v>
+      <c r="D20" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -1225,16 +1334,16 @@
       <c r="C21" t="s">
         <v>12</v>
       </c>
-      <c r="D21" t="s">
-        <v>33</v>
+      <c r="D21" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -1242,16 +1351,16 @@
       <c r="C22" t="s">
         <v>12</v>
       </c>
-      <c r="D22" t="s">
-        <v>33</v>
+      <c r="D22" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -1259,16 +1368,16 @@
       <c r="C23" t="s">
         <v>12</v>
       </c>
-      <c r="D23" t="s">
-        <v>33</v>
+      <c r="D23" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -1276,16 +1385,16 @@
       <c r="C24" t="s">
         <v>12</v>
       </c>
-      <c r="D24" t="s">
-        <v>33</v>
+      <c r="D24" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -1293,16 +1402,16 @@
       <c r="C25" t="s">
         <v>12</v>
       </c>
-      <c r="D25" t="s">
-        <v>33</v>
+      <c r="D25" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -1310,16 +1419,16 @@
       <c r="C26" t="s">
         <v>12</v>
       </c>
-      <c r="D26" t="s">
-        <v>33</v>
+      <c r="D26" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -1327,16 +1436,16 @@
       <c r="C27" t="s">
         <v>12</v>
       </c>
-      <c r="D27" t="s">
-        <v>33</v>
+      <c r="D27" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -1344,16 +1453,16 @@
       <c r="C28" t="s">
         <v>12</v>
       </c>
-      <c r="D28" t="s">
-        <v>33</v>
+      <c r="D28" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -1361,16 +1470,16 @@
       <c r="C29" t="s">
         <v>12</v>
       </c>
-      <c r="D29" t="s">
-        <v>33</v>
+      <c r="D29" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -1378,16 +1487,16 @@
       <c r="C30" t="s">
         <v>12</v>
       </c>
-      <c r="D30" t="s">
-        <v>33</v>
+      <c r="D30" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -1395,16 +1504,16 @@
       <c r="C31" t="s">
         <v>12</v>
       </c>
-      <c r="D31" t="s">
-        <v>33</v>
+      <c r="D31" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -1412,16 +1521,16 @@
       <c r="C32" t="s">
         <v>12</v>
       </c>
-      <c r="D32" t="s">
-        <v>33</v>
+      <c r="D32" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -1429,16 +1538,16 @@
       <c r="C33" t="s">
         <v>12</v>
       </c>
-      <c r="D33" t="s">
-        <v>33</v>
+      <c r="D33" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -1446,16 +1555,16 @@
       <c r="C34" t="s">
         <v>12</v>
       </c>
-      <c r="D34" t="s">
-        <v>33</v>
+      <c r="D34" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -1463,16 +1572,16 @@
       <c r="C35" t="s">
         <v>12</v>
       </c>
-      <c r="D35" t="s">
-        <v>33</v>
+      <c r="D35" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -1480,16 +1589,16 @@
       <c r="C36" t="s">
         <v>12</v>
       </c>
-      <c r="D36" t="s">
-        <v>33</v>
+      <c r="D36" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -1497,16 +1606,16 @@
       <c r="C37" t="s">
         <v>12</v>
       </c>
-      <c r="D37" t="s">
-        <v>33</v>
+      <c r="D37" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -1514,16 +1623,16 @@
       <c r="C38" t="s">
         <v>12</v>
       </c>
-      <c r="D38" t="s">
-        <v>33</v>
+      <c r="D38" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -1531,16 +1640,16 @@
       <c r="C39" t="s">
         <v>12</v>
       </c>
-      <c r="D39" t="s">
-        <v>33</v>
+      <c r="D39" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
@@ -1548,16 +1657,16 @@
       <c r="C40" t="s">
         <v>12</v>
       </c>
-      <c r="D40" t="s">
-        <v>33</v>
+      <c r="D40" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
@@ -1565,16 +1674,16 @@
       <c r="C41" t="s">
         <v>12</v>
       </c>
-      <c r="D41" t="s">
-        <v>33</v>
+      <c r="D41" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
@@ -1582,16 +1691,16 @@
       <c r="C42" t="s">
         <v>12</v>
       </c>
-      <c r="D42" t="s">
-        <v>33</v>
+      <c r="D42" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
@@ -1599,16 +1708,16 @@
       <c r="C43" t="s">
         <v>12</v>
       </c>
-      <c r="D43" t="s">
-        <v>33</v>
+      <c r="D43" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
@@ -1616,16 +1725,16 @@
       <c r="C44" t="s">
         <v>12</v>
       </c>
-      <c r="D44" t="s">
-        <v>33</v>
+      <c r="D44" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -1633,16 +1742,16 @@
       <c r="C45" t="s">
         <v>12</v>
       </c>
-      <c r="D45" t="s">
-        <v>33</v>
+      <c r="D45" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
@@ -1650,16 +1759,16 @@
       <c r="C46" t="s">
         <v>12</v>
       </c>
-      <c r="D46" t="s">
-        <v>33</v>
+      <c r="D46" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
         <v>10</v>
@@ -1667,16 +1776,16 @@
       <c r="C47" t="s">
         <v>12</v>
       </c>
-      <c r="D47" t="s">
-        <v>33</v>
+      <c r="D47" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
@@ -1684,16 +1793,16 @@
       <c r="C48" t="s">
         <v>12</v>
       </c>
-      <c r="D48" t="s">
-        <v>33</v>
+      <c r="D48" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
@@ -1701,16 +1810,16 @@
       <c r="C49" t="s">
         <v>12</v>
       </c>
-      <c r="D49" t="s">
-        <v>33</v>
+      <c r="D49" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -1718,16 +1827,16 @@
       <c r="C50" t="s">
         <v>12</v>
       </c>
-      <c r="D50" t="s">
-        <v>33</v>
+      <c r="D50" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
@@ -1735,16 +1844,16 @@
       <c r="C51" t="s">
         <v>12</v>
       </c>
-      <c r="D51" t="s">
-        <v>33</v>
+      <c r="D51" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
@@ -1752,16 +1861,16 @@
       <c r="C52" t="s">
         <v>12</v>
       </c>
-      <c r="D52" t="s">
-        <v>33</v>
+      <c r="D52" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
@@ -1769,16 +1878,16 @@
       <c r="C53" t="s">
         <v>12</v>
       </c>
-      <c r="D53" t="s">
-        <v>33</v>
+      <c r="D53" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
         <v>10</v>
@@ -1786,16 +1895,16 @@
       <c r="C54" t="s">
         <v>12</v>
       </c>
-      <c r="D54" t="s">
-        <v>33</v>
+      <c r="D54" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
@@ -1803,16 +1912,16 @@
       <c r="C55" t="s">
         <v>12</v>
       </c>
-      <c r="D55" t="s">
-        <v>33</v>
+      <c r="D55" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
@@ -1820,16 +1929,16 @@
       <c r="C56" t="s">
         <v>12</v>
       </c>
-      <c r="D56" t="s">
-        <v>33</v>
+      <c r="D56" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
@@ -1837,16 +1946,16 @@
       <c r="C57" t="s">
         <v>12</v>
       </c>
-      <c r="D57" t="s">
-        <v>33</v>
+      <c r="D57" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
@@ -1854,16 +1963,16 @@
       <c r="C58" t="s">
         <v>12</v>
       </c>
-      <c r="D58" t="s">
-        <v>33</v>
+      <c r="D58" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B59" t="s">
         <v>10</v>
@@ -1871,16 +1980,16 @@
       <c r="C59" t="s">
         <v>12</v>
       </c>
-      <c r="D59" t="s">
-        <v>33</v>
+      <c r="D59" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -1888,91 +1997,212 @@
       <c r="C60" t="s">
         <v>12</v>
       </c>
-      <c r="D60" t="s">
-        <v>33</v>
+      <c r="D60" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>17</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>143</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>145</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>146</v>
+      </c>
+      <c r="B64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>155</v>
+      </c>
+      <c r="B65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>169</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>174</v>
+      </c>
+      <c r="B68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>177</v>
+      </c>
+      <c r="B69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>178</v>
+      </c>
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="E14" r:id="rId13"/>
-    <hyperlink ref="E15" r:id="rId14"/>
-    <hyperlink ref="E16" r:id="rId15"/>
-    <hyperlink ref="E17" r:id="rId16"/>
-    <hyperlink ref="E18" r:id="rId17"/>
-    <hyperlink ref="E19" r:id="rId18"/>
-    <hyperlink ref="E20" r:id="rId19"/>
-    <hyperlink ref="E21" r:id="rId20"/>
-    <hyperlink ref="E22" r:id="rId21"/>
-    <hyperlink ref="E23" r:id="rId22"/>
-    <hyperlink ref="E24" r:id="rId23"/>
-    <hyperlink ref="E25" r:id="rId24"/>
-    <hyperlink ref="E26" r:id="rId25"/>
-    <hyperlink ref="E27" r:id="rId26"/>
-    <hyperlink ref="E28" r:id="rId27"/>
-    <hyperlink ref="E29" r:id="rId28"/>
-    <hyperlink ref="E30" r:id="rId29"/>
-    <hyperlink ref="E31" r:id="rId30"/>
-    <hyperlink ref="E32" r:id="rId31"/>
-    <hyperlink ref="E33" r:id="rId32"/>
-    <hyperlink ref="E34" r:id="rId33"/>
-    <hyperlink ref="E35" r:id="rId34"/>
-    <hyperlink ref="E36" r:id="rId35"/>
-    <hyperlink ref="E37" r:id="rId36"/>
-    <hyperlink ref="E38" r:id="rId37"/>
-    <hyperlink ref="E39" r:id="rId38"/>
-    <hyperlink ref="E40" r:id="rId39"/>
-    <hyperlink ref="E41" r:id="rId40"/>
-    <hyperlink ref="E42" r:id="rId41"/>
-    <hyperlink ref="E43" r:id="rId42"/>
-    <hyperlink ref="E44" r:id="rId43"/>
-    <hyperlink ref="E45" r:id="rId44"/>
-    <hyperlink ref="E46" r:id="rId45"/>
-    <hyperlink ref="E47" r:id="rId46"/>
-    <hyperlink ref="E48" r:id="rId47"/>
-    <hyperlink ref="E49" r:id="rId48"/>
-    <hyperlink ref="E50" r:id="rId49"/>
-    <hyperlink ref="E51" r:id="rId50"/>
-    <hyperlink ref="E52" r:id="rId51"/>
-    <hyperlink ref="E53" r:id="rId52"/>
-    <hyperlink ref="E54" r:id="rId53"/>
-    <hyperlink ref="E55" r:id="rId54"/>
-    <hyperlink ref="E56" r:id="rId55"/>
-    <hyperlink ref="E57" r:id="rId56"/>
-    <hyperlink ref="E58" r:id="rId57"/>
-    <hyperlink ref="E59" r:id="rId58"/>
-    <hyperlink ref="E60" r:id="rId59"/>
+    <hyperlink ref="E15" r:id="rId1"/>
+    <hyperlink ref="E2:E14" r:id="rId2" display="Kony@567"/>
+    <hyperlink ref="E16:E65" r:id="rId3" display="Test@546"/>
+    <hyperlink ref="E9" r:id="rId4"/>
+    <hyperlink ref="E66" r:id="rId5"/>
+    <hyperlink ref="E67" r:id="rId6"/>
+    <hyperlink ref="E68" r:id="rId7"/>
+    <hyperlink ref="E69" r:id="rId8"/>
+    <hyperlink ref="E70" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId60"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="62.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2000,18 +2230,18 @@
         <v>14</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>66</v>
+        <v>159</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
@@ -2023,18 +2253,18 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>66</v>
+        <v>159</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>8</v>
@@ -2045,19 +2275,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>66</v>
+        <v>159</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -2065,19 +2295,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>66</v>
+        <v>159</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -2085,19 +2315,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>66</v>
+        <v>159</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -2105,7 +2335,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -2117,71 +2347,71 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -2189,173 +2419,232 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>128</v>
-      </c>
       <c r="B22" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>174</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E24" t="s">
+        <v>173</v>
+      </c>
+      <c r="F24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>177</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2367,8 +2656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2387,253 +2676,256 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>165</v>
       </c>
       <c r="G5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="K5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
-        <v>108</v>
+        <v>183</v>
       </c>
       <c r="H8" t="s">
+        <v>95</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="K9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" t="s">
         <v>102</v>
       </c>
-      <c r="J10" t="s">
-        <v>109</v>
-      </c>
       <c r="K10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" t="s">
         <v>102</v>
       </c>
-      <c r="J11" t="s">
-        <v>109</v>
-      </c>
       <c r="K11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J12" t="s">
         <v>102</v>
       </c>
-      <c r="J12" t="s">
-        <v>109</v>
-      </c>
       <c r="K12" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2646,16 +2938,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2663,59 +2956,96 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>126</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2725,10 +3055,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,63 +3076,162 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>141</v>
+      <c r="D1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>